<commit_message>
Add script to run KDI biomass simulation
</commit_message>
<xml_diff>
--- a/energy_data/xlsx_data/KDI_elasticity_data.xlsx
+++ b/energy_data/xlsx_data/KDI_elasticity_data.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="21">
   <si>
     <t>Commodity</t>
   </si>
@@ -65,13 +65,25 @@
   </si>
   <si>
     <t>Natural Gas</t>
+  </si>
+  <si>
+    <t>Bernstein and Griffin</t>
+  </si>
+  <si>
+    <t>"Regional Differences in the Price-Elasticity of Demand for Energy" - RAND, NREL</t>
+  </si>
+  <si>
+    <t>average residential elasticity is -0.2811, commercial elasticity is -0.96044</t>
+  </si>
+  <si>
+    <t>Dahl and Serner</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,6 +99,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -96,10 +116,41 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -108,9 +159,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,7 +482,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,7 +491,10 @@
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="4" width="13.28515625" customWidth="1"/>
     <col min="5" max="5" width="20.140625" customWidth="1"/>
-    <col min="6" max="9" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -449,13 +516,13 @@
       <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -476,7 +543,7 @@
         <f>IF(D2=C2,"demand_own_price","demand_cross_price")</f>
         <v>demand_own_price</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="3">
         <v>-0.03</v>
       </c>
     </row>
@@ -497,7 +564,7 @@
         <f t="shared" ref="E3:E26" si="0">IF(D3=C3,"demand_own_price","demand_cross_price")</f>
         <v>demand_cross_price</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>0.51</v>
       </c>
     </row>
@@ -518,7 +585,7 @@
         <f t="shared" si="0"/>
         <v>demand_cross_price</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="3">
         <v>-0.83</v>
       </c>
     </row>
@@ -539,7 +606,7 @@
         <f t="shared" si="0"/>
         <v>demand_cross_price</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="3">
         <v>4.18</v>
       </c>
     </row>
@@ -560,7 +627,7 @@
         <f t="shared" si="0"/>
         <v>demand_cross_price</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="3">
         <v>-1.55</v>
       </c>
     </row>
@@ -581,7 +648,7 @@
         <f t="shared" si="0"/>
         <v>demand_cross_price</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="3">
         <v>0.09</v>
       </c>
     </row>
@@ -602,7 +669,7 @@
         <f t="shared" si="0"/>
         <v>demand_own_price</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="3">
         <v>-0.16</v>
       </c>
     </row>
@@ -623,7 +690,7 @@
         <f t="shared" si="0"/>
         <v>demand_cross_price</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="3">
         <v>0.04</v>
       </c>
     </row>
@@ -644,7 +711,7 @@
         <f t="shared" si="0"/>
         <v>demand_cross_price</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="3">
         <v>-1.01</v>
       </c>
     </row>
@@ -665,7 +732,7 @@
         <f t="shared" si="0"/>
         <v>demand_cross_price</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="3">
         <v>0.26</v>
       </c>
     </row>
@@ -686,9 +753,10 @@
         <f t="shared" si="0"/>
         <v>demand_cross_price</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="3">
         <v>-0.03</v>
       </c>
+      <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -707,9 +775,10 @@
         <f t="shared" si="0"/>
         <v>demand_cross_price</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="3">
         <v>0.05</v>
       </c>
+      <c r="I13" s="7"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -728,8 +797,17 @@
         <f t="shared" si="0"/>
         <v>demand_own_price</v>
       </c>
-      <c r="F14">
-        <v>-0.19</v>
+      <c r="F14" s="4">
+        <v>-0.28211111111111103</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -749,9 +827,10 @@
         <f t="shared" si="0"/>
         <v>demand_cross_price</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="3">
         <v>0.04</v>
       </c>
+      <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -770,11 +849,12 @@
         <f t="shared" si="0"/>
         <v>demand_cross_price</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="3">
         <v>-0.03</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I16" s="7"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -791,11 +871,12 @@
         <f t="shared" si="0"/>
         <v>demand_cross_price</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="3">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I17" s="7"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -812,11 +893,12 @@
         <f t="shared" si="0"/>
         <v>demand_cross_price</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="3">
         <v>-0.01</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I18" s="7"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -833,11 +915,12 @@
         <f t="shared" si="0"/>
         <v>demand_cross_price</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="3">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I19" s="7"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -854,11 +937,12 @@
         <f t="shared" si="0"/>
         <v>demand_own_price</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="3">
         <v>-0.56999999999999995</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I20" s="7"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -875,11 +959,12 @@
         <f t="shared" si="0"/>
         <v>demand_cross_price</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="3">
         <v>5.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I21" s="7"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -896,11 +981,12 @@
         <f t="shared" si="0"/>
         <v>demand_cross_price</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="3">
         <v>-6.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I22" s="7"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -917,11 +1003,12 @@
         <f t="shared" si="0"/>
         <v>demand_cross_price</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="3">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I23" s="7"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -938,11 +1025,12 @@
         <f t="shared" si="0"/>
         <v>demand_cross_price</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="3">
         <v>4.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I24" s="7"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
@@ -959,11 +1047,12 @@
         <f t="shared" si="0"/>
         <v>demand_cross_price</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="3">
         <v>3.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I25" s="7"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
@@ -980,11 +1069,14 @@
         <f t="shared" si="0"/>
         <v>demand_own_price</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="3">
         <v>-0.47</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I26" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1000,14 +1092,15 @@
       <c r="E27" t="s">
         <v>10</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="3">
         <v>0</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G27" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I27" s="7"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1023,11 +1116,12 @@
       <c r="E28" t="s">
         <v>10</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="3">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I28" s="7"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1043,11 +1137,11 @@
       <c r="E29" t="s">
         <v>10</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="3">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1063,14 +1157,14 @@
       <c r="E30" t="s">
         <v>10</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="3">
         <v>0</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1</v>
       </c>
@@ -1086,11 +1180,12 @@
       <c r="E31" t="s">
         <v>10</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="3">
         <v>0.28999999999999998</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update KDI simulation scripts
- add biofuel simulation
- commodity shock collection now includes source of energy
</commit_message>
<xml_diff>
--- a/energy_data/xlsx_data/KDI_elasticity_data.xlsx
+++ b/energy_data/xlsx_data/KDI_elasticity_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="22">
   <si>
     <t>Commodity</t>
   </si>
@@ -73,10 +73,13 @@
     <t>"Regional Differences in the Price-Elasticity of Demand for Energy" - RAND, NREL</t>
   </si>
   <si>
-    <t>average residential elasticity is -0.2811, commercial elasticity is -0.96044</t>
-  </si>
-  <si>
     <t>Dahl and Serner</t>
+  </si>
+  <si>
+    <t>average elasticity is -0.5755, max is -1.05, min is -0.16</t>
+  </si>
+  <si>
+    <t>average residential elasticity is -0.2811 (0.0753), commercial elasticity is -0.96044 (0.627)</t>
   </si>
 </sst>
 </file>
@@ -481,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,7 +804,7 @@
         <v>-0.28211111111111103</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>18</v>
@@ -1070,10 +1073,13 @@
         <v>demand_own_price</v>
       </c>
       <c r="F26" s="3">
-        <v>-0.47</v>
+        <v>-0.57550000000000001</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Change data references from gasoline to fuel
- more accurately represents code and data
</commit_message>
<xml_diff>
--- a/energy_data/xlsx_data/KDI_elasticity_data.xlsx
+++ b/energy_data/xlsx_data/KDI_elasticity_data.xlsx
@@ -43,9 +43,6 @@
     <t>Diesel</t>
   </si>
   <si>
-    <t>Gasoline</t>
-  </si>
-  <si>
     <t>supply_own_price</t>
   </si>
   <si>
@@ -80,6 +77,9 @@
   </si>
   <si>
     <t>average residential elasticity is -0.2811 (0.0753), commercial elasticity is -0.96044 (0.627)</t>
+  </si>
+  <si>
+    <t>Fuel</t>
   </si>
 </sst>
 </file>
@@ -485,7 +485,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,10 +502,10 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -520,7 +520,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>4</v>
@@ -534,7 +534,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -555,13 +555,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E26" si="0">IF(D3=C3,"demand_own_price","demand_cross_price")</f>
@@ -576,7 +576,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -597,7 +597,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -618,13 +618,13 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
@@ -639,10 +639,10 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
@@ -660,13 +660,13 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="1" t="str">
         <f t="shared" si="0"/>
@@ -681,10 +681,10 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -702,10 +702,10 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
         <v>8</v>
@@ -723,13 +723,13 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
@@ -744,7 +744,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
@@ -766,13 +766,13 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
@@ -788,7 +788,7 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
@@ -804,13 +804,13 @@
         <v>-0.28211111111111103</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -818,7 +818,7 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
@@ -840,13 +840,13 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="0"/>
@@ -862,7 +862,7 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -884,13 +884,13 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="0"/>
@@ -906,7 +906,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
@@ -928,7 +928,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
@@ -950,13 +950,13 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="0"/>
@@ -972,10 +972,10 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D22" t="s">
         <v>6</v>
@@ -994,13 +994,13 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C23" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="0"/>
@@ -1016,10 +1016,10 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C24" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D24" t="s">
         <v>7</v>
@@ -1038,10 +1038,10 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C25" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D25" t="s">
         <v>8</v>
@@ -1060,13 +1060,13 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C26" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D26" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E26" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1076,10 +1076,10 @@
         <v>-0.57550000000000001</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1087,7 +1087,7 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C27" t="s">
         <v>6</v>
@@ -1096,13 +1096,13 @@
         <v>6</v>
       </c>
       <c r="E27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F27" s="3">
         <v>0</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I27" s="7"/>
     </row>
@@ -1111,16 +1111,16 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" s="3">
         <v>0.05</v>
@@ -1132,7 +1132,7 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C29" t="s">
         <v>7</v>
@@ -1141,7 +1141,7 @@
         <v>7</v>
       </c>
       <c r="E29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29" s="3">
         <v>7.0000000000000007E-2</v>
@@ -1152,7 +1152,7 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C30" t="s">
         <v>8</v>
@@ -1161,13 +1161,13 @@
         <v>8</v>
       </c>
       <c r="E30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F30" s="3">
         <v>0</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1175,16 +1175,16 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" t="s">
         <v>9</v>
-      </c>
-      <c r="D31" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" t="s">
-        <v>10</v>
       </c>
       <c r="F31" s="3">
         <v>0.28999999999999998</v>

</xml_diff>

<commit_message>
Clear cross elasticities from KDI data
</commit_message>
<xml_diff>
--- a/energy_data/xlsx_data/KDI_elasticity_data.xlsx
+++ b/energy_data/xlsx_data/KDI_elasticity_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="23">
   <si>
     <t>Commodity</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>Fuel</t>
+  </si>
+  <si>
+    <t>elasti</t>
   </si>
 </sst>
 </file>
@@ -482,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,7 +503,7 @@
     <col min="9" max="9" width="13.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -529,7 +532,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -550,7 +553,7 @@
         <v>-0.03</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -568,10 +571,10 @@
         <v>demand_cross_price</v>
       </c>
       <c r="F3" s="3">
-        <v>0.51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -589,10 +592,10 @@
         <v>demand_cross_price</v>
       </c>
       <c r="F4" s="3">
-        <v>-0.83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -610,10 +613,10 @@
         <v>demand_cross_price</v>
       </c>
       <c r="F5" s="3">
-        <v>4.18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -631,10 +634,10 @@
         <v>demand_cross_price</v>
       </c>
       <c r="F6" s="3">
-        <v>-1.55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -652,10 +655,10 @@
         <v>demand_cross_price</v>
       </c>
       <c r="F7" s="3">
-        <v>0.09</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -676,7 +679,7 @@
         <v>-0.16</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -694,10 +697,10 @@
         <v>demand_cross_price</v>
       </c>
       <c r="F9" s="3">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -715,10 +718,10 @@
         <v>demand_cross_price</v>
       </c>
       <c r="F10" s="3">
-        <v>-1.01</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -736,10 +739,10 @@
         <v>demand_cross_price</v>
       </c>
       <c r="F11" s="3">
-        <v>0.26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -757,11 +760,11 @@
         <v>demand_cross_price</v>
       </c>
       <c r="F12" s="3">
-        <v>-0.03</v>
+        <v>0</v>
       </c>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -779,11 +782,11 @@
         <v>demand_cross_price</v>
       </c>
       <c r="F13" s="3">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="I13" s="7"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -812,8 +815,11 @@
       <c r="I14" s="7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -831,11 +837,11 @@
         <v>demand_cross_price</v>
       </c>
       <c r="F15" s="3">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -853,7 +859,7 @@
         <v>demand_cross_price</v>
       </c>
       <c r="F16" s="3">
-        <v>-0.03</v>
+        <v>0</v>
       </c>
       <c r="I16" s="7"/>
     </row>
@@ -875,7 +881,7 @@
         <v>demand_cross_price</v>
       </c>
       <c r="F17" s="3">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="I17" s="7"/>
     </row>
@@ -897,7 +903,7 @@
         <v>demand_cross_price</v>
       </c>
       <c r="F18" s="3">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="I18" s="7"/>
     </row>
@@ -919,7 +925,7 @@
         <v>demand_cross_price</v>
       </c>
       <c r="F19" s="3">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="I19" s="7"/>
     </row>
@@ -963,7 +969,7 @@
         <v>demand_cross_price</v>
       </c>
       <c r="F21" s="3">
-        <v>5.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="I21" s="7"/>
     </row>
@@ -985,7 +991,7 @@
         <v>demand_cross_price</v>
       </c>
       <c r="F22" s="3">
-        <v>-6.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="I22" s="7"/>
     </row>
@@ -1007,7 +1013,7 @@
         <v>demand_cross_price</v>
       </c>
       <c r="F23" s="3">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="I23" s="7"/>
     </row>
@@ -1029,7 +1035,7 @@
         <v>demand_cross_price</v>
       </c>
       <c r="F24" s="3">
-        <v>4.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="I24" s="7"/>
     </row>
@@ -1051,7 +1057,7 @@
         <v>demand_cross_price</v>
       </c>
       <c r="F25" s="3">
-        <v>3.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="I25" s="7"/>
     </row>

</xml_diff>